<commit_message>
correct the publishment year of SRDCF
</commit_message>
<xml_diff>
--- a/tracker_info.xlsx
+++ b/tracker_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LFL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Codes\V4R-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4518B1-A7A5-4542-A414-82A80A95219A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E92F28-E48B-4DCA-A408-DF55FBDCD106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{C441B9FF-4C92-4C38-A750-4B62B25F2E1C}"/>
   </bookViews>
@@ -526,290 +526,17 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00FF00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
+  <dxfs count="45">
     <dxf>
       <font>
         <b/>
@@ -1437,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344AEF8-CE67-457B-91B4-E75724CA4415}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1453,22 +1180,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="33" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1809,7 +1536,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>15</v>
@@ -2454,37 +2181,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="33" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -5954,167 +5681,167 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="X27:X53">
-    <cfRule type="expression" dxfId="83" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>X27=LARGE(X$27:X$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>X27=LARGE(X$27:X$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="3">
+    <cfRule type="expression" dxfId="42" priority="3">
       <formula>X27=LARGE(X$27:X$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AC3">
-    <cfRule type="expression" dxfId="44" priority="43">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>C3=LARGE($C3:$AC3,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="40" priority="44">
       <formula>C3=LARGE($C3:$AC3,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="45">
+    <cfRule type="expression" dxfId="39" priority="45">
       <formula>C3=LARGE($C3:$AC3,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AC20">
-    <cfRule type="expression" dxfId="41" priority="40">
+    <cfRule type="expression" dxfId="38" priority="40">
       <formula>C4=LARGE($C4:$AC4,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="37" priority="41">
       <formula>C4=LARGE($C4:$AC4,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="42">
+    <cfRule type="expression" dxfId="36" priority="42">
       <formula>C4=LARGE($C4:$AC4,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B53">
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>B27=LARGE(B$27:B$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="34" priority="38">
       <formula>B27=LARGE(B$27:B$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="39">
+    <cfRule type="expression" dxfId="33" priority="39">
       <formula>B27=LARGE(B$27:B$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C53">
-    <cfRule type="expression" dxfId="35" priority="34">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>C27=LARGE(C$27:C$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="31" priority="35">
       <formula>C27=LARGE(C$27:C$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="36">
+    <cfRule type="expression" dxfId="30" priority="36">
       <formula>C27=LARGE(C$27:C$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:G53">
-    <cfRule type="expression" dxfId="32" priority="31">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>F27=LARGE(F$27:F$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>F27=LARGE(F$27:F$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>F27=LARGE(F$27:F$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:K53">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>J27=LARGE(J$27:J$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>J27=LARGE(J$27:J$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>J27=LARGE(J$27:J$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27:O53">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>N27=LARGE(N$27:N$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>N27=LARGE(N$27:N$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="21" priority="27">
       <formula>N27=LARGE(N$27:N$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R27:S53">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>R27=LARGE(R$27:R$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="19" priority="23">
       <formula>R27=LARGE(R$27:R$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="18" priority="24">
       <formula>R27=LARGE(R$27:R$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V27:W53">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>V27=LARGE(V$27:V$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>V27=LARGE(V$27:V$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="15" priority="21">
       <formula>V27=LARGE(V$27:V$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D53">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>D27=LARGE(D$27:D$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>D27=LARGE(D$27:D$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>D27=LARGE(D$27:D$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H53">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>H27=LARGE(H$27:H$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>H27=LARGE(H$27:H$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>H27=LARGE(H$27:H$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:L53">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>L27=LARGE(L$27:L$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>L27=LARGE(L$27:L$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>L27=LARGE(L$27:L$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P53">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>P27=LARGE(P$27:P$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>P27=LARGE(P$27:P$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>P27=LARGE(P$27:P$53,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T27:T53">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>T27=LARGE(T$27:T$53,3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>T27=LARGE(T$27:T$53,2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>T27=LARGE(T$27:T$53,1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>